<commit_message>
Success UCFormat (Chấm công)
</commit_message>
<xml_diff>
--- a/Phân tích/UseCases/Use-Case-Format.xlsx
+++ b/Phân tích/UseCases/Use-Case-Format.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\CNPM\Phân tích\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A110E53-4E4B-46A2-BE69-C3DF126961BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777C911B-E746-4B24-91C7-99C9F20EFC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6456" yWindow="2880" windowWidth="17280" windowHeight="8964" xr2:uid="{70C1F1DC-1DC4-47AB-BCD1-D42F388C200A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{70C1F1DC-1DC4-47AB-BCD1-D42F388C200A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="UCFormat -QLNV" sheetId="1" r:id="rId1"/>
+    <sheet name="UCFormat - Chấm công" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t>Use Case Number:</t>
   </si>
@@ -284,12 +285,81 @@
   <si>
     <t>Kim Long</t>
   </si>
+  <si>
+    <t>Chấm công</t>
+  </si>
+  <si>
+    <t>Chấm công cho nhân viên dựa theo lịch làm của nhân viên</t>
+  </si>
+  <si>
+    <t>Actor action</t>
+  </si>
+  <si>
+    <t>System respone</t>
+  </si>
+  <si>
+    <t>1. Chọn menu Chấm công</t>
+  </si>
+  <si>
+    <t>2. Hệ thống hiển thị bảng chấm dựa theo nhân viên trong danh sách nhân viên</t>
+  </si>
+  <si>
+    <t>3. Hệ thống tự tính giờ theo ca làm của nhân viên dựa theo mỗi nhân viên và hiện ra màn hình</t>
+  </si>
+  <si>
+    <t>5. Hệ thống hiện ra bảng lương và số ca làm của nhân viên trong tháng</t>
+  </si>
+  <si>
+    <t>4. Quản lí chọn nhân viên và bấm mở thông tin ca làm của nhân viên đó để kiểm tra</t>
+  </si>
+  <si>
+    <t>7. Hệ thống hiện ra thông báo {xác nhận lương nhân viên thành công}</t>
+  </si>
+  <si>
+    <t>6. Quản lí chọn xác nhận tính lương. A1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>1. Quản lí chọn sửa công làm</t>
+  </si>
+  <si>
+    <t>2. Hệ thống hiện ra bảng công của nhân viên đó có thể sửa</t>
+  </si>
+  <si>
+    <t>3. Quản lí xóa hoặc thêm ca làm trong bảng công làm cho nhân viên dựa theo lịch check in</t>
+  </si>
+  <si>
+    <t>4. Quản lí chọn xác nhận</t>
+  </si>
+  <si>
+    <t>5. Hệ thống Return to step 6.</t>
+  </si>
+  <si>
+    <t>Quản lí có thể sửa ca làm (xóa, thêm hoặc chỉnh sửa) dựa theo giờ làm thực của nhân viên</t>
+  </si>
+  <si>
+    <t>Actor có đủ quyền hạn</t>
+  </si>
+  <si>
+    <t>Quản lí cần phải đăng nhập để dùng chức năng này</t>
+  </si>
+  <si>
+    <t>Ca làm cần phải được tạo ra</t>
+  </si>
+  <si>
+    <t>Chấm công vào 20 hàng tháng, ca làm tối thiểu 4 tiếng và tối đa 8 tiếng</t>
+  </si>
+  <si>
+    <t>20/11/2020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +378,32 @@
       <color theme="1"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -317,7 +413,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -403,11 +499,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -433,36 +591,89 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,65 +990,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C2621A-69EC-42B6-924F-E3471F86D7A7}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" style="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="16"/>
+    </row>
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -847,71 +1058,71 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:3" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
@@ -919,62 +1130,62 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
       <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
+    <row r="22" spans="1:3" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="16" t="s">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
@@ -982,61 +1193,61 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
+    <row r="26" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
+    <row r="27" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
+    <row r="28" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
       <c r="B28" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
+    <row r="29" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
       <c r="B29" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
       <c r="B30" s="2"/>
       <c r="C30" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
+    <row r="31" spans="1:3" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-    </row>
-    <row r="33" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="16" t="s">
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
+    <row r="34" spans="1:3" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
@@ -1044,47 +1255,47 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
+    <row r="35" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
       <c r="B35" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
+    <row r="36" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
       <c r="B36" s="6"/>
       <c r="C36" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-    </row>
-    <row r="38" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
+    <row r="37" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="17"/>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="16" t="s">
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="17"/>
-    </row>
-    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>19</v>
       </c>
@@ -1093,7 +1304,7 @@
       </c>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>20</v>
       </c>
@@ -1102,7 +1313,7 @@
       </c>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>21</v>
       </c>
@@ -1111,7 +1322,7 @@
       </c>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>23</v>
       </c>
@@ -1120,7 +1331,7 @@
       </c>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>28</v>
       </c>
@@ -1129,7 +1340,7 @@
       </c>
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1138,7 +1349,7 @@
       </c>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>30</v>
       </c>
@@ -1147,7 +1358,7 @@
       </c>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>31</v>
       </c>
@@ -1158,11 +1369,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A15:A37"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B3:C3"/>
@@ -1174,18 +1390,321 @@
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A6:A13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A15:A37"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A38:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734B381B-EDB8-4874-9EC9-0431D31E0CB1}">
+  <dimension ref="A1:C47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="79" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="24"/>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="24"/>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="24"/>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
+      <c r="B7" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="25"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="25"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="32"/>
+    </row>
+    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="24"/>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="30"/>
+      <c r="B19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="24"/>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="30"/>
+      <c r="B20" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="24"/>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="37"/>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="40"/>
+    </row>
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+    </row>
+    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="24"/>
+    </row>
+    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="24"/>
+    </row>
+    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="24"/>
+    </row>
+    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="24"/>
+    </row>
+    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="24"/>
+    </row>
+    <row r="30" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="24"/>
+    </row>
+    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="24"/>
+    </row>
+    <row r="32" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="24"/>
+    </row>
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+    </row>
+    <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+    </row>
+    <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+    </row>
+    <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+    </row>
+    <row r="37" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+    </row>
+    <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A15:A21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>